<commit_message>
Add date handling errors
</commit_message>
<xml_diff>
--- a/1-Data-errors.xlsx
+++ b/1-Data-errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irene\Dropbox (Personal)\PhD\Data-Analysis\Stanford-Geothermal-Python-Sessons--Intermediate-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D967B9-D0C9-4D78-A569-4A09B54E3439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAD1402-14C5-4CFE-BE94-747F1F708082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="707" yWindow="707" windowWidth="23693" windowHeight="11360" xr2:uid="{DE886709-EAD6-419B-A70C-CBF1C5DE4632}"/>
   </bookViews>
@@ -75,8 +75,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,8 +111,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,14 +430,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="9.5859375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.05859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.5">
@@ -466,10 +467,10 @@
       <c r="A2" s="1">
         <v>43985</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>43985</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>43896</v>
       </c>
       <c r="D2">
@@ -489,10 +490,10 @@
       <c r="A3" s="1">
         <v>43986</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>43986</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>43927</v>
       </c>
       <c r="D3">
@@ -512,10 +513,10 @@
       <c r="A4" s="1">
         <v>44015</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>44015</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>43897</v>
       </c>
       <c r="D4">
@@ -532,10 +533,10 @@
       <c r="A5" s="1">
         <v>43994</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>43994</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>44171</v>
       </c>
       <c r="D5">
@@ -558,10 +559,10 @@
       <c r="A6" s="1">
         <v>43924</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>43924</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>43894</v>
       </c>
       <c r="D6">

</xml_diff>